<commit_message>
new regressions for murray data after fixing Grrece typo
</commit_message>
<xml_diff>
--- a/analysis/paper-2013-10/table1-2-regression/V31/SI_Table13_Murray_all.xlsx
+++ b/analysis/paper-2013-10/table1-2-regression/V31/SI_Table13_Murray_all.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="14320" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="14320" tabRatio="500" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Murray_Format" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="119">
   <si>
     <t/>
   </si>
@@ -425,46 +425,49 @@
     <t>IN</t>
   </si>
   <si>
-    <t>-7.164***</t>
-  </si>
-  <si>
-    <t>0.935***</t>
-  </si>
-  <si>
-    <t>0.624***</t>
-  </si>
-  <si>
-    <t>-7.528**</t>
-  </si>
-  <si>
-    <t>0.932***</t>
-  </si>
-  <si>
-    <t>0.971***</t>
-  </si>
-  <si>
-    <t>0.568**</t>
-  </si>
-  <si>
-    <t>1.648***</t>
-  </si>
-  <si>
-    <t>1.729**</t>
-  </si>
-  <si>
-    <t>2.044**</t>
-  </si>
-  <si>
-    <t>2.286***</t>
-  </si>
-  <si>
-    <t>1.396*</t>
-  </si>
-  <si>
-    <t>2.491***</t>
-  </si>
-  <si>
-    <t>1.533**</t>
+    <t>-7.167***</t>
+  </si>
+  <si>
+    <t>0.987***</t>
+  </si>
+  <si>
+    <t>0.702***</t>
+  </si>
+  <si>
+    <t>0.412*</t>
+  </si>
+  <si>
+    <t>-7.677***</t>
+  </si>
+  <si>
+    <t>0.910***</t>
+  </si>
+  <si>
+    <t>0.964***</t>
+  </si>
+  <si>
+    <t>0.576*</t>
+  </si>
+  <si>
+    <t>0.596***</t>
+  </si>
+  <si>
+    <t>1.666***</t>
+  </si>
+  <si>
+    <t>1.778***</t>
+  </si>
+  <si>
+    <t>1.975**</t>
+  </si>
+  <si>
+    <t>2.169***</t>
+  </si>
+  <si>
+    <t>2.387***</t>
+  </si>
+  <si>
+    <t>1.321**</t>
   </si>
 </sst>
 </file>
@@ -1891,22 +1894,22 @@
       </c>
       <c r="B6" s="23" t="str">
         <f>Regression_Orig!B4</f>
-        <v>0.932***</v>
+        <v>0.910***</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
       <c r="F6" s="23" t="str">
         <f>Regression_Orig!F4</f>
-        <v>0.971***</v>
-      </c>
-      <c r="G6" s="23">
+        <v>0.964***</v>
+      </c>
+      <c r="G6" s="23" t="str">
         <f>Regression_Orig!G4</f>
-        <v>0.46899999999999997</v>
+        <v>0.576*</v>
       </c>
       <c r="H6" s="23" t="str">
         <f>Regression_Orig!H4</f>
-        <v>0.568**</v>
+        <v>0.596***</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1915,22 +1918,22 @@
       </c>
       <c r="B7" s="6">
         <f>Regression_Orig!B5</f>
-        <v>-0.13400000000000001</v>
+        <v>-0.11799999999999999</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6">
         <f>Regression_Orig!F5</f>
-        <v>-0.19600000000000001</v>
+        <v>-0.17100000000000001</v>
       </c>
       <c r="G7" s="6">
         <f>Regression_Orig!G5</f>
-        <v>-0.247</v>
+        <v>-0.223</v>
       </c>
       <c r="H7" s="6">
         <f>Regression_Orig!H5</f>
-        <v>-0.17</v>
+        <v>-0.15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17">
@@ -1939,22 +1942,22 @@
       </c>
       <c r="B8" s="23" t="str">
         <f>Regression_Orig!B6</f>
-        <v>1.648***</v>
+        <v>1.666***</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23" t="str">
         <f>Regression_Orig!F6</f>
-        <v>1.729**</v>
+        <v>1.778***</v>
       </c>
       <c r="G8" s="23">
         <f>Regression_Orig!G6</f>
-        <v>0.53300000000000003</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="H8" s="23">
         <f>Regression_Orig!H6</f>
-        <v>0.60199999999999998</v>
+        <v>0.76400000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1963,22 +1966,22 @@
       </c>
       <c r="B9" s="6">
         <f>Regression_Orig!B7</f>
-        <v>-0.377</v>
+        <v>-0.33</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6">
         <f>Regression_Orig!F7</f>
-        <v>-0.48299999999999998</v>
+        <v>-0.42099999999999999</v>
       </c>
       <c r="G9" s="6">
         <f>Regression_Orig!G7</f>
-        <v>-0.621</v>
+        <v>-0.56100000000000005</v>
       </c>
       <c r="H9" s="6">
         <f>Regression_Orig!H7</f>
-        <v>-0.48399999999999999</v>
+        <v>-0.42599999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1988,13 +1991,13 @@
       <c r="B10" s="23"/>
       <c r="C10" s="23" t="str">
         <f>Regression_Orig!C8</f>
-        <v>2.044**</v>
+        <v>1.975**</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23">
         <f>Regression_Orig!F8</f>
-        <v>-0.17199999999999999</v>
+        <v>-0.24</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
@@ -2006,13 +2009,13 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6">
         <f>Regression_Orig!C9</f>
-        <v>-0.58399999999999996</v>
+        <v>-0.54600000000000004</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6">
         <f>Regression_Orig!F9</f>
-        <v>-0.624</v>
+        <v>-0.54500000000000004</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -2025,13 +2028,13 @@
       <c r="C12" s="23"/>
       <c r="D12" s="23" t="str">
         <f>Regression_Orig!D10</f>
-        <v>2.286***</v>
+        <v>2.169***</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="23" t="str">
+      <c r="G12" s="23">
         <f>Regression_Orig!G10</f>
-        <v>1.396*</v>
+        <v>1.006</v>
       </c>
       <c r="H12" s="23"/>
     </row>
@@ -2043,13 +2046,13 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6">
         <f>Regression_Orig!D11</f>
-        <v>-0.33</v>
+        <v>-0.31</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6">
         <f>Regression_Orig!G11</f>
-        <v>-0.64100000000000001</v>
+        <v>-0.57899999999999996</v>
       </c>
       <c r="H13" s="6"/>
     </row>
@@ -2062,13 +2065,13 @@
       <c r="D14" s="23"/>
       <c r="E14" s="23" t="str">
         <f>Regression_Orig!E12</f>
-        <v>2.491***</v>
+        <v>2.387***</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
       <c r="H14" s="23" t="str">
         <f>Regression_Orig!H12</f>
-        <v>1.533**</v>
+        <v>1.321**</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2078,13 +2081,13 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6">
         <f>Regression_Orig!E13</f>
-        <v>-0.40500000000000003</v>
+        <v>-0.375</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6">
         <f>Regression_Orig!H13</f>
-        <v>-0.51900000000000002</v>
+        <v>-0.45700000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2093,62 +2096,62 @@
       </c>
       <c r="B16" s="23" t="str">
         <f>Regression_Orig!B2</f>
-        <v>-7.164***</v>
+        <v>-7.167***</v>
       </c>
       <c r="C16" s="23" t="str">
         <f>Regression_Orig!C2</f>
-        <v>0.935***</v>
+        <v>0.987***</v>
       </c>
       <c r="D16" s="23" t="str">
         <f>Regression_Orig!D2</f>
-        <v>0.624***</v>
-      </c>
-      <c r="E16" s="23">
+        <v>0.702***</v>
+      </c>
+      <c r="E16" s="23" t="str">
         <f>Regression_Orig!E2</f>
-        <v>0.33</v>
+        <v>0.412*</v>
       </c>
       <c r="F16" s="23" t="str">
         <f>Regression_Orig!F2</f>
-        <v>-7.528**</v>
+        <v>-7.677***</v>
       </c>
       <c r="G16" s="23">
         <f>Regression_Orig!G2</f>
-        <v>-2.1190000000000002</v>
+        <v>-3.532</v>
       </c>
       <c r="H16" s="23">
         <f>Regression_Orig!H2</f>
-        <v>-2.766</v>
+        <v>-3.3759999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="8"/>
       <c r="B17" s="5">
         <f>Regression_Orig!B3</f>
-        <v>-1.7509999999999999</v>
+        <v>-1.532</v>
       </c>
       <c r="C17" s="5">
         <f>Regression_Orig!C3</f>
-        <v>-0.20499999999999999</v>
+        <v>-0.192</v>
       </c>
       <c r="D17" s="5">
         <f>Regression_Orig!D3</f>
-        <v>-0.156</v>
+        <v>-0.14699999999999999</v>
       </c>
       <c r="E17" s="5">
         <f>Regression_Orig!E3</f>
-        <v>-0.214</v>
+        <v>-0.19800000000000001</v>
       </c>
       <c r="F17" s="5">
         <f>Regression_Orig!F3</f>
-        <v>-2.222</v>
+        <v>-1.9390000000000001</v>
       </c>
       <c r="G17" s="5">
         <f>Regression_Orig!G3</f>
-        <v>-2.835</v>
+        <v>-2.5579999999999998</v>
       </c>
       <c r="H17" s="5">
         <f>Regression_Orig!H3</f>
-        <v>-2.1360000000000001</v>
+        <v>-1.879</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2194,7 +2197,7 @@
       </c>
       <c r="C19" s="3">
         <f>Regression_Orig!C18</f>
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D19" s="3">
         <f>Regression_Orig!D18</f>
@@ -2223,31 +2226,31 @@
       </c>
       <c r="B20" s="3">
         <f>Regression_Orig!B15</f>
-        <v>0.66200000000000003</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="C20" s="3">
         <f>Regression_Orig!C15</f>
-        <v>0.32</v>
+        <v>0.33400000000000002</v>
       </c>
       <c r="D20" s="3">
         <f>Regression_Orig!D15</f>
-        <v>0.64900000000000002</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="E20" s="3">
         <f>Regression_Orig!E15</f>
-        <v>0.59299999999999997</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="F20" s="3">
         <f>Regression_Orig!F15</f>
-        <v>0.66300000000000003</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="G20" s="3">
         <f>Regression_Orig!G15</f>
-        <v>0.71799999999999997</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="H20" s="3">
         <f>Regression_Orig!H15</f>
-        <v>0.752</v>
+        <v>0.78600000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2256,31 +2259,31 @@
       </c>
       <c r="B21" s="16">
         <f>Regression_Orig!B16</f>
-        <v>0.63500000000000001</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="C21" s="16">
         <f>Regression_Orig!C16</f>
-        <v>0.29399999999999998</v>
+        <v>0.309</v>
       </c>
       <c r="D21" s="16">
         <f>Regression_Orig!D16</f>
-        <v>0.63600000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="E21" s="16">
         <f>Regression_Orig!E16</f>
-        <v>0.57699999999999996</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="F21" s="16">
         <f>Regression_Orig!F16</f>
-        <v>0.621</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="G21" s="16">
         <f>Regression_Orig!G16</f>
-        <v>0.68300000000000005</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="H21" s="16">
         <f>Regression_Orig!H16</f>
-        <v>0.72099999999999997</v>
+        <v>0.75900000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="7" customHeight="1">
@@ -2381,22 +2384,22 @@
       </c>
       <c r="B6" s="23" t="str">
         <f>Regression_Orig!B4</f>
-        <v>0.932***</v>
+        <v>0.910***</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
       <c r="F6" s="23" t="str">
         <f>Regression_Orig!F4</f>
-        <v>0.971***</v>
-      </c>
-      <c r="G6" s="23">
+        <v>0.964***</v>
+      </c>
+      <c r="G6" s="23" t="str">
         <f>Regression_Orig!G4</f>
-        <v>0.46899999999999997</v>
+        <v>0.576*</v>
       </c>
       <c r="H6" s="23" t="str">
         <f>Regression_Orig!H4</f>
-        <v>0.568**</v>
+        <v>0.596***</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2405,22 +2408,22 @@
       </c>
       <c r="B7" s="6">
         <f>Regression_Orig!B5</f>
-        <v>-0.13400000000000001</v>
+        <v>-0.11799999999999999</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6">
         <f>Regression_Orig!F5</f>
-        <v>-0.19600000000000001</v>
+        <v>-0.17100000000000001</v>
       </c>
       <c r="G7" s="6">
         <f>Regression_Orig!G5</f>
-        <v>-0.247</v>
+        <v>-0.223</v>
       </c>
       <c r="H7" s="6">
         <f>Regression_Orig!H5</f>
-        <v>-0.17</v>
+        <v>-0.15</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17">
@@ -2429,22 +2432,22 @@
       </c>
       <c r="B8" s="23" t="str">
         <f>Regression_Orig!B6</f>
-        <v>1.648***</v>
+        <v>1.666***</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23" t="str">
         <f>Regression_Orig!F6</f>
-        <v>1.729**</v>
+        <v>1.778***</v>
       </c>
       <c r="G8" s="23">
         <f>Regression_Orig!G6</f>
-        <v>0.53300000000000003</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="H8" s="23">
         <f>Regression_Orig!H6</f>
-        <v>0.60199999999999998</v>
+        <v>0.76400000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2453,22 +2456,22 @@
       </c>
       <c r="B9" s="6">
         <f>Regression_Orig!B7</f>
-        <v>-0.377</v>
+        <v>-0.33</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6">
         <f>Regression_Orig!F7</f>
-        <v>-0.48299999999999998</v>
+        <v>-0.42099999999999999</v>
       </c>
       <c r="G9" s="6">
         <f>Regression_Orig!G7</f>
-        <v>-0.621</v>
+        <v>-0.56100000000000005</v>
       </c>
       <c r="H9" s="6">
         <f>Regression_Orig!H7</f>
-        <v>-0.48399999999999999</v>
+        <v>-0.42599999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2478,13 +2481,13 @@
       <c r="B10" s="23"/>
       <c r="C10" s="23" t="str">
         <f>Regression_Orig!C8</f>
-        <v>2.044**</v>
+        <v>1.975**</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23">
         <f>Regression_Orig!F8</f>
-        <v>-0.17199999999999999</v>
+        <v>-0.24</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
@@ -2496,13 +2499,13 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6">
         <f>Regression_Orig!C9</f>
-        <v>-0.58399999999999996</v>
+        <v>-0.54600000000000004</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6">
         <f>Regression_Orig!F9</f>
-        <v>-0.624</v>
+        <v>-0.54500000000000004</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -2515,13 +2518,13 @@
       <c r="C12" s="23"/>
       <c r="D12" s="23" t="str">
         <f>Regression_Orig!D10</f>
-        <v>2.286***</v>
+        <v>2.169***</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="23" t="str">
+      <c r="G12" s="23">
         <f>Regression_Orig!G10</f>
-        <v>1.396*</v>
+        <v>1.006</v>
       </c>
       <c r="H12" s="23"/>
     </row>
@@ -2533,13 +2536,13 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6">
         <f>Regression_Orig!D11</f>
-        <v>-0.33</v>
+        <v>-0.31</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6">
         <f>Regression_Orig!G11</f>
-        <v>-0.64100000000000001</v>
+        <v>-0.57899999999999996</v>
       </c>
       <c r="H13" s="6"/>
     </row>
@@ -2552,13 +2555,13 @@
       <c r="D14" s="23"/>
       <c r="E14" s="23" t="str">
         <f>Regression_Orig!E12</f>
-        <v>2.491***</v>
+        <v>2.387***</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
       <c r="H14" s="23" t="str">
         <f>Regression_Orig!H12</f>
-        <v>1.533**</v>
+        <v>1.321**</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2568,13 +2571,13 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6">
         <f>Regression_Orig!E13</f>
-        <v>-0.40500000000000003</v>
+        <v>-0.375</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6">
         <f>Regression_Orig!H13</f>
-        <v>-0.51900000000000002</v>
+        <v>-0.45700000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2583,62 +2586,62 @@
       </c>
       <c r="B16" s="23" t="str">
         <f>Regression_Orig!B2</f>
-        <v>-7.164***</v>
+        <v>-7.167***</v>
       </c>
       <c r="C16" s="23" t="str">
         <f>Regression_Orig!C2</f>
-        <v>0.935***</v>
+        <v>0.987***</v>
       </c>
       <c r="D16" s="23" t="str">
         <f>Regression_Orig!D2</f>
-        <v>0.624***</v>
-      </c>
-      <c r="E16" s="23">
+        <v>0.702***</v>
+      </c>
+      <c r="E16" s="23" t="str">
         <f>Regression_Orig!E2</f>
-        <v>0.33</v>
+        <v>0.412*</v>
       </c>
       <c r="F16" s="23" t="str">
         <f>Regression_Orig!F2</f>
-        <v>-7.528**</v>
+        <v>-7.677***</v>
       </c>
       <c r="G16" s="23">
         <f>Regression_Orig!G2</f>
-        <v>-2.1190000000000002</v>
+        <v>-3.532</v>
       </c>
       <c r="H16" s="23">
         <f>Regression_Orig!H2</f>
-        <v>-2.766</v>
+        <v>-3.3759999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="8"/>
       <c r="B17" s="5">
         <f>Regression_Orig!B3</f>
-        <v>-1.7509999999999999</v>
+        <v>-1.532</v>
       </c>
       <c r="C17" s="5">
         <f>Regression_Orig!C3</f>
-        <v>-0.20499999999999999</v>
+        <v>-0.192</v>
       </c>
       <c r="D17" s="5">
         <f>Regression_Orig!D3</f>
-        <v>-0.156</v>
+        <v>-0.14699999999999999</v>
       </c>
       <c r="E17" s="5">
         <f>Regression_Orig!E3</f>
-        <v>-0.214</v>
+        <v>-0.19800000000000001</v>
       </c>
       <c r="F17" s="5">
         <f>Regression_Orig!F3</f>
-        <v>-2.222</v>
+        <v>-1.9390000000000001</v>
       </c>
       <c r="G17" s="5">
         <f>Regression_Orig!G3</f>
-        <v>-2.835</v>
+        <v>-2.5579999999999998</v>
       </c>
       <c r="H17" s="5">
         <f>Regression_Orig!H3</f>
-        <v>-2.1360000000000001</v>
+        <v>-1.879</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2684,7 +2687,7 @@
       </c>
       <c r="C19" s="3">
         <f>Regression_Orig!C18</f>
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D19" s="3">
         <f>Regression_Orig!D18</f>
@@ -2713,31 +2716,31 @@
       </c>
       <c r="B20" s="3">
         <f>Regression_Orig!B15</f>
-        <v>0.66200000000000003</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="C20" s="3">
         <f>Regression_Orig!C15</f>
-        <v>0.32</v>
+        <v>0.33400000000000002</v>
       </c>
       <c r="D20" s="3">
         <f>Regression_Orig!D15</f>
-        <v>0.64900000000000002</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="E20" s="3">
         <f>Regression_Orig!E15</f>
-        <v>0.59299999999999997</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="F20" s="3">
         <f>Regression_Orig!F15</f>
-        <v>0.66300000000000003</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="G20" s="3">
         <f>Regression_Orig!G15</f>
-        <v>0.71799999999999997</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="H20" s="3">
         <f>Regression_Orig!H15</f>
-        <v>0.752</v>
+        <v>0.78600000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2746,31 +2749,31 @@
       </c>
       <c r="B21" s="16">
         <f>Regression_Orig!B16</f>
-        <v>0.63500000000000001</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="C21" s="16">
         <f>Regression_Orig!C16</f>
-        <v>0.29399999999999998</v>
+        <v>0.309</v>
       </c>
       <c r="D21" s="16">
         <f>Regression_Orig!D16</f>
-        <v>0.63600000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="E21" s="16">
         <f>Regression_Orig!E16</f>
-        <v>0.57699999999999996</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="F21" s="16">
         <f>Regression_Orig!F16</f>
-        <v>0.621</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="G21" s="16">
         <f>Regression_Orig!G16</f>
-        <v>0.68300000000000005</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="H21" s="16">
         <f>Regression_Orig!H16</f>
-        <v>0.72099999999999997</v>
+        <v>0.75900000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="7" customHeight="1">
@@ -2799,8 +2802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2851,17 +2854,17 @@
       <c r="D2" t="s">
         <v>106</v>
       </c>
-      <c r="E2">
-        <v>0.33</v>
+      <c r="E2" t="s">
+        <v>107</v>
       </c>
       <c r="F2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G2">
-        <v>-2.1190000000000002</v>
+        <v>-3.532</v>
       </c>
       <c r="H2">
-        <v>-2.766</v>
+        <v>-3.3759999999999999</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
@@ -2873,25 +2876,25 @@
     </row>
     <row r="3" spans="1:15">
       <c r="B3">
-        <v>-1.7509999999999999</v>
+        <v>-1.532</v>
       </c>
       <c r="C3">
-        <v>-0.20499999999999999</v>
+        <v>-0.192</v>
       </c>
       <c r="D3">
-        <v>-0.156</v>
+        <v>-0.14699999999999999</v>
       </c>
       <c r="E3">
-        <v>-0.214</v>
+        <v>-0.19800000000000001</v>
       </c>
       <c r="F3">
-        <v>-2.222</v>
+        <v>-1.9390000000000001</v>
       </c>
       <c r="G3">
-        <v>-2.835</v>
+        <v>-2.5579999999999998</v>
       </c>
       <c r="H3">
-        <v>-2.1360000000000001</v>
+        <v>-1.879</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -2906,16 +2909,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4">
-        <v>0.46899999999999997</v>
+        <v>110</v>
+      </c>
+      <c r="G4" t="s">
+        <v>111</v>
       </c>
       <c r="H4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
@@ -2927,16 +2930,16 @@
     </row>
     <row r="5" spans="1:15">
       <c r="B5">
-        <v>-0.13400000000000001</v>
+        <v>-0.11799999999999999</v>
       </c>
       <c r="F5">
-        <v>-0.19600000000000001</v>
+        <v>-0.17100000000000001</v>
       </c>
       <c r="G5">
-        <v>-0.247</v>
+        <v>-0.223</v>
       </c>
       <c r="H5">
-        <v>-0.17</v>
+        <v>-0.15</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -2951,16 +2954,16 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G6">
-        <v>0.53300000000000003</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="H6">
-        <v>0.60199999999999998</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -2972,16 +2975,16 @@
     </row>
     <row r="7" spans="1:15">
       <c r="B7">
-        <v>-0.377</v>
+        <v>-0.33</v>
       </c>
       <c r="F7">
-        <v>-0.48299999999999998</v>
+        <v>-0.42099999999999999</v>
       </c>
       <c r="G7">
-        <v>-0.621</v>
+        <v>-0.56100000000000005</v>
       </c>
       <c r="H7">
-        <v>-0.48399999999999999</v>
+        <v>-0.42599999999999999</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -2996,10 +2999,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F8">
-        <v>-0.17199999999999999</v>
+        <v>-0.24</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -3011,10 +3014,10 @@
     </row>
     <row r="9" spans="1:15">
       <c r="C9">
-        <v>-0.58399999999999996</v>
+        <v>-0.54600000000000004</v>
       </c>
       <c r="F9">
-        <v>-0.624</v>
+        <v>-0.54500000000000004</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -3029,10 +3032,10 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
-      </c>
-      <c r="G10" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="G10">
+        <v>1.006</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -3044,10 +3047,10 @@
     </row>
     <row r="11" spans="1:15">
       <c r="D11">
-        <v>-0.33</v>
+        <v>-0.31</v>
       </c>
       <c r="G11">
-        <v>-0.64100000000000001</v>
+        <v>-0.57899999999999996</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -3062,10 +3065,10 @@
         <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -3077,10 +3080,10 @@
     </row>
     <row r="13" spans="1:15">
       <c r="E13">
-        <v>-0.40500000000000003</v>
+        <v>-0.375</v>
       </c>
       <c r="H13">
-        <v>-0.51900000000000002</v>
+        <v>-0.45700000000000002</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -3095,25 +3098,25 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0.495</v>
+        <v>0.433</v>
       </c>
       <c r="C14">
-        <v>0.68799999999999994</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="D14">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="E14">
         <v>0.49399999999999999</v>
       </c>
-      <c r="E14">
-        <v>0.53300000000000003</v>
-      </c>
       <c r="F14">
-        <v>0.504</v>
+        <v>0.44</v>
       </c>
       <c r="G14">
-        <v>0.46100000000000002</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="H14">
-        <v>0.432</v>
+        <v>0.38</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
@@ -3128,25 +3131,25 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>0.66200000000000003</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="C15">
-        <v>0.32</v>
+        <v>0.33400000000000002</v>
       </c>
       <c r="D15">
-        <v>0.64900000000000002</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="E15">
-        <v>0.59299999999999997</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="F15">
-        <v>0.66300000000000003</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="G15">
-        <v>0.71799999999999997</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="H15">
-        <v>0.752</v>
+        <v>0.78600000000000003</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -3161,25 +3164,25 @@
         <v>26</v>
       </c>
       <c r="B16">
-        <v>0.63500000000000001</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="C16">
-        <v>0.29399999999999998</v>
+        <v>0.309</v>
       </c>
       <c r="D16">
-        <v>0.63600000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="E16">
-        <v>0.57699999999999996</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="F16">
-        <v>0.621</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="G16">
-        <v>0.68300000000000005</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="H16">
-        <v>0.72099999999999997</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -3194,25 +3197,25 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>24.513000000000002</v>
+        <v>30.736999999999998</v>
       </c>
       <c r="C17">
-        <v>12.259</v>
+        <v>13.061</v>
       </c>
       <c r="D17">
-        <v>48.112000000000002</v>
+        <v>48.911000000000001</v>
       </c>
       <c r="E17">
-        <v>37.847999999999999</v>
+        <v>40.454999999999998</v>
       </c>
       <c r="F17">
-        <v>15.763</v>
+        <v>19.896000000000001</v>
       </c>
       <c r="G17">
-        <v>20.367999999999999</v>
+        <v>23.155000000000001</v>
       </c>
       <c r="H17">
-        <v>24.291</v>
+        <v>29.32</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
@@ -3230,7 +3233,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3303,7 +3306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -3624,7 +3627,7 @@
       </c>
       <c r="C26" s="27">
         <f>Top10_Orig!B14</f>
-        <v>0.69345841902274497</v>
+        <v>0.69345841902274596</v>
       </c>
       <c r="D26" s="18"/>
     </row>
@@ -3638,7 +3641,7 @@
       </c>
       <c r="C27" s="27">
         <f>Top10_Orig!B15</f>
-        <v>0.570558612190604</v>
+        <v>0.570558612190605</v>
       </c>
       <c r="D27" s="18"/>
     </row>
@@ -3652,7 +3655,7 @@
       </c>
       <c r="C28" s="27">
         <f>Top10_Orig!B16</f>
-        <v>0.50814412819499899</v>
+        <v>0.50814412819499999</v>
       </c>
       <c r="D28" s="18"/>
     </row>
@@ -3680,7 +3683,7 @@
       </c>
       <c r="C30" s="27">
         <f>Top10_Orig!B18</f>
-        <v>0.47336187734823898</v>
+        <v>0.47336187734823998</v>
       </c>
       <c r="D30" s="18"/>
     </row>
@@ -3734,7 +3737,7 @@
       </c>
       <c r="C35" s="27">
         <f>Top10_Orig!B25</f>
-        <v>0.88185388582830704</v>
+        <v>0.88185388582830904</v>
       </c>
       <c r="D35" s="18"/>
     </row>
@@ -3748,7 +3751,7 @@
       </c>
       <c r="C36" s="27">
         <f>Top10_Orig!B26</f>
-        <v>0.818472173093031</v>
+        <v>0.818472173093032</v>
       </c>
       <c r="D36" s="18"/>
     </row>
@@ -3762,7 +3765,7 @@
       </c>
       <c r="C37" s="27">
         <f>Top10_Orig!B27</f>
-        <v>0.72286681675426601</v>
+        <v>0.72286681675426701</v>
       </c>
       <c r="D37" s="18"/>
     </row>
@@ -3776,7 +3779,7 @@
       </c>
       <c r="C38" s="27">
         <f>Top10_Orig!B28</f>
-        <v>0.71678019423930694</v>
+        <v>0.71678019423930805</v>
       </c>
       <c r="D38" s="18"/>
     </row>
@@ -3840,7 +3843,7 @@
       </c>
       <c r="C44" s="30">
         <f>Top10_Orig!B36</f>
-        <v>0.94857366116124298</v>
+        <v>0.94857366116124198</v>
       </c>
       <c r="D44" s="18"/>
     </row>
@@ -3854,7 +3857,7 @@
       </c>
       <c r="C45" s="30">
         <f>Top10_Orig!B37</f>
-        <v>0.90848577814725595</v>
+        <v>0.90848577814725495</v>
       </c>
       <c r="D45" s="18"/>
     </row>
@@ -3868,7 +3871,7 @@
       </c>
       <c r="C46" s="30">
         <f>Top10_Orig!B38</f>
-        <v>0.85798762905557702</v>
+        <v>0.85798762905557502</v>
       </c>
       <c r="D46" s="18"/>
     </row>
@@ -3882,7 +3885,7 @@
       </c>
       <c r="C47" s="30">
         <f>Top10_Orig!B39</f>
-        <v>0.77715725912947198</v>
+        <v>0.77715725912947098</v>
       </c>
       <c r="D47" s="18"/>
     </row>
@@ -3936,8 +3939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B12" sqref="A1:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4047,7 +4050,7 @@
         <v>55</v>
       </c>
       <c r="B14" s="10">
-        <v>0.69345841902274497</v>
+        <v>0.69345841902274596</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4055,7 +4058,7 @@
         <v>58</v>
       </c>
       <c r="B15" s="10">
-        <v>0.570558612190604</v>
+        <v>0.570558612190605</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4063,7 +4066,7 @@
         <v>53</v>
       </c>
       <c r="B16" s="10">
-        <v>0.50814412819499899</v>
+        <v>0.50814412819499999</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4079,7 +4082,7 @@
         <v>56</v>
       </c>
       <c r="B18" s="10">
-        <v>0.47336187734823898</v>
+        <v>0.47336187734823998</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4103,7 +4106,7 @@
         <v>84</v>
       </c>
       <c r="B21" s="10">
-        <v>0.31745817998435</v>
+        <v>0.317458179984351</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4133,7 +4136,7 @@
         <v>54</v>
       </c>
       <c r="B25" s="10">
-        <v>0.88185388582830704</v>
+        <v>0.88185388582830904</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4141,7 +4144,7 @@
         <v>53</v>
       </c>
       <c r="B26" s="10">
-        <v>0.818472173093031</v>
+        <v>0.818472173093032</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4149,7 +4152,7 @@
         <v>55</v>
       </c>
       <c r="B27" s="10">
-        <v>0.72286681675426601</v>
+        <v>0.72286681675426701</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4157,7 +4160,7 @@
         <v>65</v>
       </c>
       <c r="B28" s="10">
-        <v>0.71678019423930694</v>
+        <v>0.71678019423930805</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4189,7 +4192,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="10">
-        <v>0.58223225610346196</v>
+        <v>0.58223225610346296</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4219,7 +4222,7 @@
         <v>54</v>
       </c>
       <c r="B36" s="10">
-        <v>0.94857366116124298</v>
+        <v>0.94857366116124198</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4227,7 +4230,7 @@
         <v>53</v>
       </c>
       <c r="B37" s="10">
-        <v>0.90848577814725595</v>
+        <v>0.90848577814725495</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -4235,7 +4238,7 @@
         <v>57</v>
       </c>
       <c r="B38" s="10">
-        <v>0.85798762905557702</v>
+        <v>0.85798762905557502</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4243,7 +4246,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="10">
-        <v>0.77715725912947198</v>
+        <v>0.77715725912947098</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4267,7 +4270,7 @@
         <v>61</v>
       </c>
       <c r="B42" s="10">
-        <v>0.54718586642552602</v>
+        <v>0.54718586642552502</v>
       </c>
     </row>
     <row r="43" spans="1:2">

</xml_diff>